<commit_message>
SQL project in progress
</commit_message>
<xml_diff>
--- a/Excel/nifty_500.xlsx
+++ b/Excel/nifty_500.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kinnari\Desktop\Data_Analysis\Tableau\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kinnari\Desktop\Data_Analysis\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9491C48-60F4-4C73-8E64-629D583F419A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DCDBCD-35FF-4934-8622-3C2803A678A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nifty_500" sheetId="1" r:id="rId1"/>
@@ -3154,7 +3154,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3989,12 +3989,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q502"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24.54296875" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" customWidth="1"/>
+    <col min="7" max="7" width="13.7265625" customWidth="1"/>
+    <col min="8" max="8" width="15.90625" customWidth="1"/>
+    <col min="9" max="9" width="14.81640625" customWidth="1"/>
+    <col min="10" max="10" width="12.6328125" customWidth="1"/>
+    <col min="11" max="11" width="15.6328125" customWidth="1"/>
+    <col min="12" max="12" width="18.1796875" customWidth="1"/>
+    <col min="13" max="13" width="18.7265625" customWidth="1"/>
+    <col min="17" max="17" width="19.90625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>